<commit_message>
added the activity types file and modified the list
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Referentiels-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29790B5F-C562-4C7B-85D5-1B9012BB8F06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847D338-76C1-44AC-9CC2-52B7ED611734}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>Référentiel des domaines fonctionnels et fonctions des collectivités</t>
   </si>
   <si>
-    <t>Référentiel produit à partir du RI_104 du SIA et surtout de sa version enrichie de définitions, d'exemples et d'alignements, et organisée hiérarchiquement produite à l'aide de Ginco. 35 entités dotées de définitions, 32 dotées d'exemples, 7 alignées sur des entités Wkidata.</t>
-  </si>
-  <si>
     <t>Référentiel produit à partir du RI_011 du SIA et surtout de sa version enrichie de nouvelles entités et organisée hiérarchiquement, en cours de construction à l'aide de Ginco. 35 entités ayant le statut de candidat. 56 entités dotées de définitions.</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
       </rPr>
       <t>. Le tableau sera mis à jour avec les référentiels. SIA signifie : Système d'Information Archivistique des Archives nationales. 'skos:' désigne l'espace de noms du vocabulaire SKOS (Simple Knowledge Organization System), http://www.w3.org/2004/02/skos/core# . 'rico:' désigne l'espace de noms de l'ontologie Records in Contexts-Ontology, https://www.ica.org/standards/RiC/ontology#.</t>
     </r>
+  </si>
+  <si>
+    <t>Référentiel produit à partir du RI_104 du SIA et surtout de sa version enrichie de définitions, d'exemples et d'alignements, et organisée hiérarchiquement produite à l'aide de Ginco. 35 entités dotées de définitions, 32 dotées d'exemples, 7 alignées sur des entités Wikidata.</t>
   </si>
 </sst>
 </file>
@@ -344,12 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -358,6 +352,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30889D5F-EB5E-44C5-9923-9945B5CA472C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,30 +685,30 @@
     <col min="2" max="2" width="70.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="44" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
     <col min="7" max="7" width="68.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -723,7 +723,7 @@
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -742,9 +742,9 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
@@ -759,9 +759,9 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,7 +772,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>50</v>
@@ -780,7 +780,7 @@
       <c r="D6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>15210</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -803,7 +803,7 @@
       <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -826,7 +826,7 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>240</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -849,7 +849,7 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -872,7 +872,7 @@
       <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -895,7 +895,7 @@
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -918,7 +918,7 @@
       <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -941,7 +941,7 @@
       <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -964,7 +964,7 @@
       <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>2219</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -987,7 +987,7 @@
       <c r="D15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>380</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1010,14 +1010,14 @@
       <c r="D16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>190</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1033,14 +1033,14 @@
       <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
       <c r="D18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="D19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
added a few details in the list file
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847D338-76C1-44AC-9CC2-52B7ED611734}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB6F237-3A4D-421C-A292-FBC65C0D9255}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Nom du référentiel</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>rico:Person; rico:Family; rico:CorporateBody; rico:CorporateBodyType; rico:OccupationType; rico:ActivityType; rico:Relation et ses sous-classes</t>
-  </si>
-  <si>
-    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utlisant RiC-O Converter, qui regroupe et déduplique les relations. Un fichier par agent, et plusieurs fichiers pour les relations. Fourni avec une liste au format tsv (en utf-8; séparateur : tabulation) des producteurs</t>
   </si>
   <si>
     <t>skos:Concept; rico:ActivityType</t>
@@ -264,6 +261,21 @@
   </si>
   <si>
     <t>Référentiel produit à partir du RI_104 du SIA et surtout de sa version enrichie de définitions, d'exemples et d'alignements, et organisée hiérarchiquement produite à l'aide de Ginco. 35 entités dotées de définitions, 32 dotées d'exemples, 7 alignées sur des entités Wikidata.</t>
+  </si>
+  <si>
+    <t>Référentiel dit des personnes morales</t>
+  </si>
+  <si>
+    <t>Référentiel dit des personnes physiques</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_013 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 40 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
+  </si>
+  <si>
+    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant RiC-O Converter, qui regroupe et déduplique les relations EAC-CPF. Un fichier par agent, et plusieurs fichiers pour les relations. Fourni avec une liste au format tsv (en utf-8; séparateur : tabulation) des producteurs</t>
   </si>
 </sst>
 </file>
@@ -675,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30889D5F-EB5E-44C5-9923-9945B5CA472C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -733,46 +745,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="E4" s="7">
+        <v>487</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2134</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>50</v>
@@ -787,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -999,25 +1023,25 @@
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="7">
         <v>190</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1037,10 +1061,10 @@
         <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1058,7 +1082,7 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>

<commit_message>
added the first persons and corporate bodies data, changed the list file
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB6F237-3A4D-421C-A292-FBC65C0D9255}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F496BF-09F4-4BD5-B3A4-3B97B037192B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>agents/producteurs</t>
   </si>
   <si>
-    <t>agents/personnesMorales</t>
-  </si>
-  <si>
     <t>agents/personnesPhysiques</t>
   </si>
   <si>
@@ -269,13 +266,16 @@
     <t>Référentiel dit des personnes physiques</t>
   </si>
   <si>
-    <t>Référentiel produit automatiquement à partir du RI_013 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 40 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
-  </si>
-  <si>
     <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant RiC-O Converter, qui regroupe et déduplique les relations EAC-CPF. Un fichier par agent, et plusieurs fichiers pour les relations. Fourni avec une liste au format tsv (en utf-8; séparateur : tabulation) des producteurs</t>
+  </si>
+  <si>
+    <t>agents/collectivites</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_013 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 40 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -745,18 +745,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="7">
         <v>487</v>
@@ -765,21 +765,21 @@
         <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="7">
         <v>2134</v>
@@ -788,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -796,13 +796,13 @@
         <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="7">
         <v>15210</v>
@@ -811,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1023,25 +1023,25 @@
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="7">
         <v>190</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1061,43 +1061,43 @@
         <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">

</xml_diff>

<commit_message>
added the EAC-CPF and RDF/RiC-O files about the persons, families and corporate bodies that created the fonds held by the ANF and updated the XLSX list
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F496BF-09F4-4BD5-B3A4-3B97B037192B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC3F42C-FEC9-4698-AFF7-EDE3BC354809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Versions disponibles</t>
   </si>
   <si>
-    <t>RDF: classes utilisées</t>
-  </si>
-  <si>
     <t>Nombre d'entités décrites</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>skos:Concept; rico:CorporateBodyType</t>
   </si>
   <si>
-    <t>agents/producteurs</t>
-  </si>
-  <si>
     <t>agents/personnesPhysiques</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
   </si>
   <si>
     <t>rico:Place; rico:PhysicalLocation; rico:Coordinates; rico:PlaceType</t>
-  </si>
-  <si>
-    <t>rico:Person; rico:Family; rico:CorporateBody; rico:CorporateBodyType; rico:OccupationType; rico:ActivityType; rico:Relation et ses sous-classes</t>
   </si>
   <si>
     <t>skos:Concept; rico:ActivityType</t>
@@ -266,9 +257,6 @@
     <t>Référentiel dit des personnes physiques</t>
   </si>
   <si>
-    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant RiC-O Converter, qui regroupe et déduplique les relations EAC-CPF. Un fichier par agent, et plusieurs fichiers pour les relations. Fourni avec une liste au format tsv (en utf-8; séparateur : tabulation) des producteurs</t>
-  </si>
-  <si>
     <t>agents/collectivites</t>
   </si>
   <si>
@@ -276,6 +264,18 @@
   </si>
   <si>
     <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
+  </si>
+  <si>
+    <t>rico:Person; rico:Family; rico:CorporateBody; rico:CorporateBodyType; rico:OccupationType; rico:ActivityType; rico:Relation et ses sous-classes ; rico:Place</t>
+  </si>
+  <si>
+    <t>agents/producteurs/eac-cpf et agents/producteurs/rdf</t>
+  </si>
+  <si>
+    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant le logiciel RiC-O Converter (https://github.com/ArchivesNationalesFR/rico-converter), et en rendant ensuite par script le résultat conforme à RiC-O 0.2. Un fichier par agent, 6 fichiers pour les relations entre agents et relations de provenance entre agents et documents, + un fichier pour les lieux (qui sera repris prochainement). Fourni avec une liste des notices EAC-CPF au format tsv (en utf-8; séparateur : tabulation). ATTENTION : les notices dont la liste TSV indique qu'elles ne contiennent pas d'éléments biographiques ou historiques rédigés (pas d'élément EAC-CPF biogHist) et/ou qu'elles ont été créées en 2013 ne sont pas forcément fiables (des vérifications et enrichissements restent à faire) ; leur version RDF ne l'est pas plus.</t>
+  </si>
+  <si>
+    <t>RDF: principales classes utilisées</t>
   </si>
 </sst>
 </file>
@@ -687,13 +687,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30889D5F-EB5E-44C5-9923-9945B5CA472C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="44" style="5" customWidth="1"/>
@@ -704,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -723,8 +723,8 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
+      <c r="A3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -733,375 +733,375 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>71</v>
+      <c r="A4" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7">
         <v>487</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
+      <c r="A5" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" s="7">
         <v>2134</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E6" s="7">
         <v>15210</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="7">
         <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E8" s="7">
         <v>240</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E9" s="7">
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="7">
         <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
+      <c r="A12" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="7">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E14" s="7">
         <v>2219</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E15" s="7">
         <v>380</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
+      <c r="A16" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E16" s="7">
         <v>190</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="7">
         <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>51</v>
+      <c r="A18" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="4"/>
     </row>

</xml_diff>

<commit_message>
fixed some properties (owl:sameAs changed to skos:exactMatch) in the place types vocab., updated the Excel list
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\prepa-referentiels-dec2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3823502B-9CFE-49AA-A15C-D285007B3908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9BADC7-CE1E-4C41-9244-3E7C1B9847A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Référentiel produit hors du SIA pour catégoriser les entités géo-historiques décrites dans le référentiel des lieux.</t>
-  </si>
-  <si>
     <t>Référentiel des types de documents</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fichiers produits à partir du RI_005 du SIA. Nombreux ajouts par rapport au fichier source (relations d'équivalence avec les entités des référentiels IGN et INSEE et pour quelques entités avec Geonames ou Wikidata, relations d'inclusion, relations d'adjacence, parfois des historiques et des relations chronologiques, parfois une description ;  coordonnées géographiques - longitude et latitude- du chef-lieu des régions et des départements et des communes). Décrivent : les communes (36776 entités), départements (168 départements anciens ou actuels) et régions (33 régions anciennes ou actuelles) français ; 132 lieux-dits en France ; 209 pays ; 606 villes ou territoires étrangers ; 367 édifices en France et à l'étranger ; 233 éléments de géographie physique. Les géométries des communes, départements et régions ne sont pas présentes dans cette version : cela aurait trop alourdi les fichiers. </t>
+  </si>
+  <si>
+    <t>Référentiel produit hors du SIA pour catégoriser les entités géo-historiques décrites dans le référentiel des lieux. 8 entités alignées avec autant d'entités des vocabulaires de l'IGN.</t>
   </si>
 </sst>
 </file>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30889D5F-EB5E-44C5-9923-9945B5CA472C}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -777,7 +777,7 @@
     </row>
     <row r="3" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -786,10 +786,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>2</v>
@@ -803,111 +803,111 @@
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="7">
         <v>487</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="7">
         <v>2134</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="7">
         <v>15210</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="7">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -916,10 +916,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="7">
         <v>67</v>
@@ -928,319 +928,319 @@
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F9" s="7">
         <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F10" s="7">
         <v>22</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="7">
         <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F15" s="7">
         <v>2219</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F16" s="7">
         <v>381</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="7">
         <v>190</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F18" s="7">
         <v>61</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="7">
         <v>38524</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="F20" s="7">
         <v>14949</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version of the list of files
</commit_message>
<xml_diff>
--- a/Liste-referentiels.xlsx
+++ b/Liste-referentiels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\Referentiels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\github-archivesnationales\referentiels-mars2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9BADC7-CE1E-4C41-9244-3E7C1B9847A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3F3891-D1C5-466C-8BB8-D7AD650440C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229F457F-D761-4B7A-BC86-EA9EDF898744}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
   <si>
     <t>Nom du référentiel</t>
   </si>
@@ -120,9 +120,6 @@
     <t>skos:Concept; rico:OccupationType</t>
   </si>
   <si>
-    <t>Référentiel produit automatiquement à partir du RI_010 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 18 entités dotées de 'définitions'.</t>
-  </si>
-  <si>
     <t>Référentiel des types de collectivités</t>
   </si>
   <si>
@@ -163,6 +160,114 @@
   </si>
   <si>
     <t>Référentiel des producteurs des fonds et séries d'archives conservés aux Archives nationales</t>
+  </si>
+  <si>
+    <t>Référentiel dit des personnes morales</t>
+  </si>
+  <si>
+    <t>Référentiel dit des personnes physiques</t>
+  </si>
+  <si>
+    <t>agents/collectivites</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_013 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 40 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
+  </si>
+  <si>
+    <t>rico:Person; rico:Family; rico:CorporateBody; rico:CorporateBodyType; rico:OccupationType; rico:ActivityType; rico:Relation et ses sous-classes ; rico:Place</t>
+  </si>
+  <si>
+    <t>agents/producteurs/eac-cpf et agents/producteurs/rdf</t>
+  </si>
+  <si>
+    <t>RDF: principales classes utilisées</t>
+  </si>
+  <si>
+    <t>Référentiel des langues des documents</t>
+  </si>
+  <si>
+    <t>rico:Language</t>
+  </si>
+  <si>
+    <t>2019; 2021-11</t>
+  </si>
+  <si>
+    <t>Référentiel produit manuellement à partir des données contenues dans la liste des langues du SIA (FRAN_RI_100). Embryonnaire et partiel (ne prend pour l'instant pas en compte la totalité des langues déclarées dans la liste SIA). Relations d'équivalence et labels ajoutés dans le fichier RDF.</t>
+  </si>
+  <si>
+    <t>2021-05;2021-11</t>
+  </si>
+  <si>
+    <t>2021-05</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_001 du SIA après marquage du type d'entité. Pas de différence notable avec le contenu du référentiel SIA. Sera enrichi de façon significative dans les prochains mois.</t>
+  </si>
+  <si>
+    <t>2019; 2021-04</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>OUI mais incomplet par rapport à la version RDF</t>
+  </si>
+  <si>
+    <t>OUI mais très incomplet par rapport à la version RDF</t>
+  </si>
+  <si>
+    <t>2021-04;2021-12</t>
+  </si>
+  <si>
+    <t>2019;2021-11</t>
+  </si>
+  <si>
+    <t>Référentiel produit hors du SIA pour catégoriser les entités géo-historiques décrites dans le référentiel des lieux. 8 entités alignées avec autant d'entités des vocabulaires de l'IGN.</t>
+  </si>
+  <si>
+    <t>2019-06-16; 2022-03</t>
+  </si>
+  <si>
+    <t>2019; 2022-05</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_001 du SIA après marquage du type d'entité. Pas de différence notable avec le contenu du référentiel SIA. 46 entités dotées de définitions actuellement.  Sera enrichi de façon significative dans les prochains mois.</t>
+  </si>
+  <si>
+    <t>2021-05;2022-05</t>
+  </si>
+  <si>
+    <t>2021-04; 2022-04</t>
+  </si>
+  <si>
+    <t>RDF : date de création; date de dernière modification du contenu</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du RI_010 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 19 entités dotées de 'définitions'.</t>
+  </si>
+  <si>
+    <t>2019; 2022-04</t>
+  </si>
+  <si>
+    <t>Référentiel produit à partir du RI_104 du SIA et surtout de sa version enrichie de définitions, d'exemples et d'alignements, et organisée hiérarchiquement produite à l'aide de Ginco. 37 entités dotées de définitions, 32 dotées d'exemples, 8 alignées sur des entités Wikidata.</t>
+  </si>
+  <si>
+    <t>Référentiel produit automatiquement à partir du thésaurus RI_004 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 433 entités dotées de 'définitions'. 497 relations d'équivalence avec des concepts d'autres référentiels (Thesaurus de la désignation des oeuvres architecturales et des espaces aménagés du MCC, BnF, Getty, DBPedia...), pour 137 entités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fichiers produits à partir des 7 fichiers correspondants dans le SIA des Archives nationales. Décrivent sommairement :  68 paroisses parisiennes avant 1789 ;  145 quartiers parisiens ; les 24 communes rattachées en totalité ou partiellement à Paris en 1860 ; les 12 arrondissements parisiens avant 1860 ; les 20 arrondissements actuels ; 1491 édifices dans les limites actuelles de Paris ; 13189 voies parisiennes du Moyen Age à nos jours. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fichiers produits à partir du RI_005 du SIA. Nombreux ajouts par rapport au fichier source (relations d'équivalence avec les entités des référentiels IGN et INSEE et pour quelques entités avec Geonames ou Wikidata, relations d'inclusion, relations d'adjacence, parfois des historiques et des relations chronologiques, parfois une description ;  coordonnées géographiques - longitude et latitude- du chef-lieu des régions et des départements et des communes). Décrivent : les communes (36778 entités, pour l'essentiel avant 2014), départements (173 départements anciens ou actuels) et régions (33 régions anciennes ou actuelles) français ; 132 lieux-dits en France ; 209 pays ; 606 villes ou territoires étrangers ; 367 édifices en France et à l'étranger ; 233 éléments de géographie physique. Les géométries des communes, départements et régions ne sont pas présentes dans cette version : cela aurait trop alourdi les fichiers. </t>
+  </si>
+  <si>
+    <t>2019;2022-04</t>
+  </si>
+  <si>
+    <t>2019; 2022-03</t>
+  </si>
+  <si>
+    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant le logiciel RiC-O Converter (https://github.com/ArchivesNationalesFR/rico-converter), et en rendant ensuite par script le résultat conforme à RiC-O 0.2. Un fichier par agent, 6 fichiers pour les relations entre agents et relations de provenance entre agents et documents, + un fichier pour les lieux). Fourni avec une liste des notices EAC-CPF au format CSV (en utf-8; séparateur : virgule ; valeurs des colonnes encadrées par des guillemets). ATTENTION : les notices dont la liste  indique qu'elles ne contiennent pas d'éléments biographiques ou historiques rédigés (pas d'élément EAC-CPF biogHist) et/ou qu'elles ont été créées en 2013 ne sont pas forcément fiables (des vérifications et enrichissements restent à faire).</t>
   </si>
   <si>
     <r>
@@ -174,7 +279,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Liste des référentiels disponibles</t>
+      <t>Liste des référentiels disponibles dans la release 1.0</t>
     </r>
     <r>
       <rPr>
@@ -184,149 +289,56 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. Le tableau sera mis à jour avec les référentiels. SIA signifie : Système d'Information Archivistique des Archives nationales. 'skos:' désigne l'espace de noms du vocabulaire SKOS (Simple Knowledge Organization System), http://www.w3.org/2004/02/skos/core# . 'rico:' désigne l'espace de noms de l'ontologie Records in Contexts-Ontology, https://www.ica.org/standards/RiC/ontology#.</t>
+      <t>. SIA signifie : Système d'Information Archivistique des Archives nationales. 'skos:' désigne l'espace de noms du vocabulaire SKOS (Simple Knowledge Organization System), http://www.w3.org/2004/02/skos/core# . 'rico:' désigne l'espace de noms de l'ontologie Records in Contexts-Ontology, https://www.ica.org/standards/RiC/ontology#.</t>
     </r>
   </si>
   <si>
-    <t>Référentiel produit à partir du RI_104 du SIA et surtout de sa version enrichie de définitions, d'exemples et d'alignements, et organisée hiérarchiquement produite à l'aide de Ginco. 35 entités dotées de définitions, 32 dotées d'exemples, 7 alignées sur des entités Wikidata.</t>
-  </si>
-  <si>
-    <t>Référentiel dit des personnes morales</t>
-  </si>
-  <si>
-    <t>Référentiel dit des personnes physiques</t>
-  </si>
-  <si>
-    <t>agents/collectivites</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_013 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 40 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs.</t>
-  </si>
-  <si>
-    <t>rico:Person; rico:Family; rico:CorporateBody; rico:CorporateBodyType; rico:OccupationType; rico:ActivityType; rico:Relation et ses sous-classes ; rico:Place</t>
-  </si>
-  <si>
-    <t>agents/producteurs/eac-cpf et agents/producteurs/rdf</t>
-  </si>
-  <si>
-    <t>RDF: principales classes utilisées</t>
-  </si>
-  <si>
-    <t>RDF : date de création; date de dernière modification</t>
-  </si>
-  <si>
-    <t>2019-06-16; 2021-03-02</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_placeTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_001_documentaryFormTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_001_recordSetTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_001_recordStates.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_002_carrierTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_002_productionTechniqueTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_002_representationTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_004_things.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_010_occupationTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_011_activityTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_RI_104_corporateBodyTypes.rdf</t>
-  </si>
-  <si>
-    <t>concepts/FRAN_languages.rdf</t>
-  </si>
-  <si>
-    <t>Référentiel des langues des documents</t>
-  </si>
-  <si>
-    <t>rico:Language</t>
-  </si>
-  <si>
-    <t>2019; 2021-11</t>
-  </si>
-  <si>
-    <t>Référentiel produit manuellement à partir des données contenues dans la liste des langues du SIA (FRAN_RI_100). Embryonnaire et partiel (ne prend pour l'instant pas en compte la totalité des langues déclarées dans la liste SIA). Relations d'équivalence et labels ajoutés dans le fichier RDF.</t>
-  </si>
-  <si>
-    <t>2019; 2021-05</t>
-  </si>
-  <si>
-    <t>Référentiel produit à partir du référentiel des producteurs du SIA, en utilisant le logiciel RiC-O Converter (https://github.com/ArchivesNationalesFR/rico-converter), et en rendant ensuite par script le résultat conforme à RiC-O 0.2. Un fichier par agent, 6 fichiers pour les relations entre agents et relations de provenance entre agents et documents, + un fichier pour les lieux). Fourni avec une liste des notices EAC-CPF au format tsv (en utf-8; séparateur : tabulation). ATTENTION : les notices dont la liste TSV indique qu'elles ne contiennent pas d'éléments biographiques ou historiques rédigés (pas d'élément EAC-CPF biogHist) et/ou qu'elles ont été créées en 2013 ne sont pas forcément fiables (des vérifications et enrichissements restent à faire) ; leur version RDF ne l'est donc pas plus.</t>
-  </si>
-  <si>
-    <t>2021-05;2021-11</t>
-  </si>
-  <si>
-    <t>2021-05</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_001 du SIA après marquage du type d'entité. Pas de différence notable avec le contenu du référentiel SIA. Sera enrichi de façon significative dans les prochains mois.</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_001 du SIA après marquage du type d'entité. Pas de différence notable avec le contenu du référentiel SIA. Une addition manuelle (skos:relatedMatch vers un type de document).  Sera enrichi de façon significative dans les prochains mois.</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du RI_001 du SIA après marquage du type d'entité. Pas de différence notable avec le contenu du référentiel SIA. 38 entités dotées de définitions actuellement. Une addition manuelle (skos:relatedMatch vers un type de groupe de document).  Sera enrichi de façon significative dans les prochains mois.</t>
-  </si>
-  <si>
-    <t>2019; 2021-04</t>
-  </si>
-  <si>
-    <t>2021-04</t>
-  </si>
-  <si>
-    <t>Référentiel produit automatiquement à partir du thésaurus RI_004 du SIA. Pas de différence notable avec le contenu du référentiel SIA. 433 entités dotées de 'définitions'. 490 relations d'équivalence avec des concepts d'autres référentiels (Thesaurus de la désignation des oeuvres architecturales du MCC, BnF, Getty, DBPedia...)</t>
-  </si>
-  <si>
-    <t>OUI mais incomplet par rapport à la version RDF</t>
-  </si>
-  <si>
-    <t>OUI mais très incomplet par rapport à la version RDF</t>
-  </si>
-  <si>
-    <t>2021-04;2021-12</t>
-  </si>
-  <si>
-    <t>2019;2021-04</t>
-  </si>
-  <si>
-    <t>lieux/lieuxHorsParis.zip</t>
-  </si>
-  <si>
-    <t>lieux/lieuxDansParis.zip (7 fichiers)</t>
-  </si>
-  <si>
-    <t>2019;2021-11</t>
-  </si>
-  <si>
-    <t>Fichiers produits à partir des 7 fichiers correspondants dans le SIA des Archives nationales. Lieux qualifiés via le référentiel des types de lieux. Décrivent :  68 paroisses parisiennes avant 1789 ;  145 quartiers parisiens ; les 24 communes rattachées en totalité ou partiellement à Paris en 1860 ; les 12 arrondissements parisiens avant 1860 ; les 20 arrondissements actuels ; 1491 édifices dans les limites actuelles de Paris ; 13189 voies parisiennes du Moyen Age à nos jours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fichiers produits à partir du RI_005 du SIA. Nombreux ajouts par rapport au fichier source (relations d'équivalence avec les entités des référentiels IGN et INSEE et pour quelques entités avec Geonames ou Wikidata, relations d'inclusion, relations d'adjacence, parfois des historiques et des relations chronologiques, parfois une description ;  coordonnées géographiques - longitude et latitude- du chef-lieu des régions et des départements et des communes). Décrivent : les communes (36776 entités), départements (168 départements anciens ou actuels) et régions (33 régions anciennes ou actuelles) français ; 132 lieux-dits en France ; 209 pays ; 606 villes ou territoires étrangers ; 367 édifices en France et à l'étranger ; 233 éléments de géographie physique. Les géométries des communes, départements et régions ne sont pas présentes dans cette version : cela aurait trop alourdi les fichiers. </t>
-  </si>
-  <si>
-    <t>Référentiel produit hors du SIA pour catégoriser les entités géo-historiques décrites dans le référentiel des lieux. 8 entités alignées avec autant d'entités des vocabulaires de l'IGN.</t>
+    <t>Référentiel produit automatiquement à partir du RI_012 du SIA. Pas de différence notable avec le contenu du référentiel SIA. Un fichier par agent. (02 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs. 102 entités alignées (owl:sameAs) avec autant d'entités du référentiel des producteurs, 205 avec des entités Wikidata, 67 avec des entités de la BnF, 61 avec des entités de la base ISNI.</t>
+  </si>
+  <si>
+    <t>RDF et CSV</t>
+  </si>
+  <si>
+    <t>concepts/csv/FRAN_RI_100_languages.csv et concepts/rdf/FRAN_languages.rdf</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_placeTypes.rdf et concepts/csv/FRAN_placeTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_001_documentaryFormTypes.rdf et concepts/csv/FRAN_RI_001_documentaryFormTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_001_recordSetTypes.rdf et concepts/csv/FRAN_RI_001_recordSetTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_002_carrierTypes.rdf et concepts/csv/FRAN_RI_002_carrierTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_001_recordStates.rdf et concepts/csv/FRAN_RI_001_recordStates.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_002_productionTechniqueTypes.rdf et concepts/csv/FRAN_RI_002_productionTechniqueTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_002_representationTypes.rdf et concepts/csv/FRAN_RI_002_representationTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_004_things.rdf et concepts/csv/FRAN_RI_004_things.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_010_occupationTypes.rdf et concepts/csv/FRAN_RI_010_occupationTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_011_activityTypes.rdf et concepts/csv/FRAN_RI_011_activityTypes.csv</t>
+  </si>
+  <si>
+    <t>concepts/rdf/FRAN_RI_104_corporateBodyTypes.rdf et concepts/csv/FRAN_RI_104_corporateBodyTypes.csv</t>
+  </si>
+  <si>
+    <t>lieux situés à Paris (fichiers lieux/rdf/FRAN_Paris_*.rdf et lieux/csv/FRAN_Paris_*.csv)</t>
+  </si>
+  <si>
+    <t>lieux situés hors de Paris (fichiers dont le nom ne contient pas 'Paris' dans lieux/rdf/ et lieux/csv/)</t>
   </si>
 </sst>
 </file>
@@ -738,13 +750,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30889D5F-EB5E-44C5-9923-9945B5CA472C}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="53" style="5" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="5" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="44" style="5" customWidth="1"/>
@@ -755,7 +767,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -786,10 +798,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>2</v>
@@ -803,19 +815,19 @@
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7">
         <v>487</v>
@@ -824,24 +836,24 @@
         <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="7">
         <v>2134</v>
@@ -850,50 +862,50 @@
         <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F6" s="7">
-        <v>15210</v>
+        <v>15484</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="F7" s="7">
         <v>10</v>
@@ -902,21 +914,21 @@
         <v>10</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
@@ -928,73 +940,73 @@
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="7">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>14</v>
@@ -1006,21 +1018,21 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>15</v>
@@ -1035,18 +1047,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>20</v>
@@ -1063,16 +1075,16 @@
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>19</v>
@@ -1087,18 +1099,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>25</v>
@@ -1110,21 +1122,21 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>27</v>
@@ -1136,102 +1148,102 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="7">
         <v>190</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F18" s="7">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="7">
+        <v>38531</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="7">
-        <v>38524</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="F20" s="7">
         <v>14949</v>
@@ -1240,7 +1252,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>